<commit_message>
+) updated .xlsx - only marked done things with green
</commit_message>
<xml_diff>
--- a/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
+++ b/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbau\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="16245" windowHeight="11760"/>
   </bookViews>
@@ -898,7 +893,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -955,6 +950,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="11" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1021,9 +1022,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1061,9 +1062,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1098,7 +1099,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1133,7 +1134,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1309,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1359,24 +1360,24 @@
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
@@ -1386,13 +1387,13 @@
       <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
@@ -1413,22 +1414,22 @@
       <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:3" s="6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" s="6" customFormat="1" ht="305.10000000000002" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">

</xml_diff>

<commit_message>
+) Arc42 template update
</commit_message>
<xml_diff>
--- a/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
+++ b/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1396,22 +1396,22 @@
       <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">

</xml_diff>

<commit_message>
- highlighted done part (Kapitel 8)
</commit_message>
<xml_diff>
--- a/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
+++ b/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MIT_SAD\2nd_sem\sad\murrent_grill_pieber_lehner\final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="16245" windowHeight="11760"/>
   </bookViews>
@@ -960,48 +965,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1022,9 +1027,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1062,9 +1067,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1099,7 +1104,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1134,7 +1139,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1310,11 +1315,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C10"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="16.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.3984375" customWidth="1"/>
     <col min="2" max="2" width="32.796875" customWidth="1"/>
@@ -1499,137 +1504,137 @@
       <c r="C19" s="13"/>
     </row>
     <row r="20" spans="1:3" s="6" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3" s="6" customFormat="1" ht="125.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="20"/>
     </row>
     <row r="31" spans="1:3" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="20" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="20" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1739,7 +1744,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+) Updated arc42 final version
</commit_message>
<xml_diff>
--- a/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
+++ b/2nd_sem/sad/murrent_grill_pieber_lehner/final/Feedback-EVA-Lehner-2014-05-30.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario\Documents\SourceTree\fhwn\MIT_SAD\2nd_sem\sad\murrent_grill_pieber_lehner\final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="16245" windowHeight="11760"/>
+    <workbookView xWindow="477" yWindow="106" windowWidth="16246" windowHeight="5548"/>
   </bookViews>
   <sheets>
     <sheet name="Itemlist" sheetId="1" r:id="rId1"/>
@@ -1016,9 +1021,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1056,9 +1061,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,7 +1098,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1128,7 +1133,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1304,18 +1309,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C16" sqref="A16:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.8125" defaultRowHeight="14.6" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" customWidth="1"/>
-    <col min="2" max="2" width="32.796875" customWidth="1"/>
-    <col min="3" max="3" width="42.59765625" customWidth="1"/>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
+    <col min="2" max="2" width="32.8125" customWidth="1"/>
+    <col min="3" max="3" width="42.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
         <v>75</v>
       </c>
@@ -1335,7 +1340,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1346,14 +1351,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:3" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>5</v>
       </c>
@@ -1364,7 +1369,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="6" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="6" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>16</v>
       </c>
@@ -1373,14 +1378,14 @@
       </c>
       <c r="C6" s="19"/>
     </row>
-    <row r="7" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="6" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1394,7 @@
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="6" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>9</v>
       </c>
@@ -1398,7 +1403,7 @@
       </c>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>9</v>
       </c>
@@ -1407,7 +1412,7 @@
       </c>
       <c r="C10" s="19"/>
     </row>
-    <row r="11" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>20</v>
       </c>
@@ -1416,7 +1421,7 @@
       </c>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:3" s="6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="6" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>23</v>
       </c>
@@ -1425,7 +1430,7 @@
       </c>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="1:3" s="6" customFormat="1" ht="305.10000000000002" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="6" customFormat="1" ht="349.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -1434,7 +1439,7 @@
       </c>
       <c r="C13" s="17"/>
     </row>
-    <row r="14" spans="1:3" s="6" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="6" customFormat="1" ht="105.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>27</v>
       </c>
@@ -1445,14 +1450,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
     </row>
-    <row r="16" spans="1:3" s="6" customFormat="1" ht="249.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="6" customFormat="1" ht="249.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>30</v>
       </c>
@@ -1463,7 +1468,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>31</v>
       </c>
@@ -1474,7 +1479,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>35</v>
       </c>
@@ -1485,14 +1490,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
     </row>
-    <row r="20" spans="1:3" s="6" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="6" customFormat="1" ht="115" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>47</v>
       </c>
@@ -1503,7 +1508,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18" t="s">
         <v>53</v>
       </c>
@@ -1512,7 +1517,7 @@
       </c>
       <c r="C21" s="18"/>
     </row>
-    <row r="22" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>48</v>
       </c>
@@ -1523,7 +1528,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>49</v>
       </c>
@@ -1534,7 +1539,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="6" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
         <v>50</v>
       </c>
@@ -1545,7 +1550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="6" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
         <v>12</v>
       </c>
@@ -1554,7 +1559,7 @@
       </c>
       <c r="C25" s="18"/>
     </row>
-    <row r="26" spans="1:3" s="6" customFormat="1" ht="125.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="6" customFormat="1" ht="125.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>51</v>
       </c>
@@ -1565,7 +1570,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="6" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>51</v>
       </c>
@@ -1574,7 +1579,7 @@
       </c>
       <c r="C27" s="18"/>
     </row>
-    <row r="28" spans="1:3" s="6" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="6" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>51</v>
       </c>
@@ -1585,7 +1590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
         <v>51</v>
       </c>
@@ -1596,7 +1601,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>51</v>
       </c>
@@ -1605,7 +1610,7 @@
       </c>
       <c r="C30" s="18"/>
     </row>
-    <row r="31" spans="1:3" s="6" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="6" customFormat="1" ht="120.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>51</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="6" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>51</v>
       </c>
@@ -1627,14 +1632,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="6" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
     </row>
-    <row r="34" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="6" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>67</v>
       </c>
@@ -1643,7 +1648,7 @@
       </c>
       <c r="C34" s="14"/>
     </row>
-    <row r="35" spans="1:3" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>69</v>
       </c>
@@ -1652,7 +1657,7 @@
       </c>
       <c r="C35" s="19"/>
     </row>
-    <row r="36" spans="1:3" s="6" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="6" customFormat="1" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
         <v>73</v>
       </c>
@@ -1663,59 +1668,59 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" s="2"/>
     </row>
   </sheetData>
@@ -1733,7 +1738,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1875" defaultRowHeight="14.6" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>